<commit_message>
Added Component-3 of Hybrid-EBM - added function 'compute_qul'
</commit_message>
<xml_diff>
--- a/Parameters-Estimation/Lx_Parameters_Estimation/0-Dataset/Lx_forecast_2016_2019_CMEMS.xlsx
+++ b/Parameters-Estimation/Lx_Parameters_Estimation/0-Dataset/Lx_forecast_2016_2019_CMEMS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\4_CMCC\Progetti\3_EBM\1_EBM_LX_SALINITY_CK_PO_GORO\Experiments\Parameters-Estimation\Lx_Parameters_Estimation\0-Dataset\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\4_CMCC\Progetti\3_EBM_EstuarIO\1_Hybrid_EBM-Po-Goro\Experiments\Parameters-Estimation\Lx_Parameters_Estimation\0-Dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1562304F-6D35-4D3A-9EEA-B059C8B6ED7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EC41B4E-C50E-467C-A79E-307D39353504}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-1800" yWindow="4845" windowWidth="21600" windowHeight="11385" xr2:uid="{7318206E-4FEC-4547-A442-A3D665FB0687}"/>
+    <workbookView xWindow="-20610" yWindow="4455" windowWidth="19680" windowHeight="11760" xr2:uid="{7318206E-4FEC-4547-A442-A3D665FB0687}"/>
   </bookViews>
   <sheets>
     <sheet name="Lx_2016_2019" sheetId="1" r:id="rId1"/>

</xml_diff>